<commit_message>
Update lecture materials and examples for SUMIF and rounding
Added new Excel files and images for function and string operations, updated and expanded MCfCL-08-Lecture.md with improved explanations and examples for SUMIF, ROUND, ROUNDDOWN, and ROUNDUP functions, and removed outdated practice files. Also added a PDF version of the lecture and new figures to support the updated content.
</commit_message>
<xml_diff>
--- a/MCfCL-08-Lecture/08_Function_sample-demo.xlsx
+++ b/MCfCL-08-Lecture/08_Function_sample-demo.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tetsu\github\2025-SIT-MCfCL\MCfCL-08-Lecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92358DDD-A2FE-4DFA-9E9C-EE98A2910F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC6A3257-D167-42AF-BA62-B277AD74D75C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="1590" windowWidth="26130" windowHeight="13890" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1110" yWindow="7020" windowWidth="27810" windowHeight="17820" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="注文履歴" sheetId="1" r:id="rId1"/>
     <sheet name="基本集計" sheetId="2" r:id="rId2"/>
     <sheet name="条件付き合計（例）" sheetId="3" r:id="rId3"/>
     <sheet name="条件付き合計" sheetId="4" r:id="rId4"/>
+    <sheet name="丸め" sheetId="5" r:id="rId5"/>
+    <sheet name="文字列操作" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="103">
   <si>
     <t>注文ID</t>
   </si>
@@ -213,114 +215,392 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>例１</t>
+    <t>スマートフォン</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>社員ID</t>
+  </si>
+  <si>
+    <t>氏名</t>
+  </si>
+  <si>
+    <t>部署</t>
+  </si>
+  <si>
+    <t>勤務日数</t>
+  </si>
+  <si>
+    <t>残業時間</t>
+  </si>
+  <si>
+    <t>E001</t>
+  </si>
+  <si>
+    <t>営業</t>
+  </si>
+  <si>
+    <t>E002</t>
+  </si>
+  <si>
+    <t>経理</t>
+  </si>
+  <si>
+    <t>E003</t>
+  </si>
+  <si>
+    <t>開発</t>
+  </si>
+  <si>
+    <t>E004</t>
+  </si>
+  <si>
+    <t>E005</t>
+  </si>
+  <si>
+    <t>E006</t>
+  </si>
+  <si>
+    <t>中村健</t>
+  </si>
+  <si>
+    <t>E007</t>
+  </si>
+  <si>
+    <t>E008</t>
+  </si>
+  <si>
+    <t>総務</t>
+  </si>
+  <si>
+    <t>E009</t>
+  </si>
+  <si>
+    <t>E010</t>
+  </si>
+  <si>
+    <t>練習内容</t>
+  </si>
+  <si>
+    <t>条件</t>
+  </si>
+  <si>
+    <t>使用関数例</t>
+  </si>
+  <si>
+    <t>結果</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> =SUMIF(D3:D12,"営業",E3:E12)</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>営業部の勤務日数合計</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>勤務日数20日以上の残業時間合計</t>
+    <rPh sb="6" eb="7">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="10" eb="12">
+      <t>ザンギョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ジカン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>20日以上</t>
+    <rPh sb="2" eb="3">
+      <t>ニチ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>イジョウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> =SUMIF(D3:D12,"開発",</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>？</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <rPh sb="16" eb="18">
+      <t>カイハツ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> =SUMIF(E3:E12,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>？</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>？</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="UD Digi Kyokasho NP-R"/>
+        <family val="1"/>
+        <charset val="128"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>開発部の残業時間合計</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>商品名が「スマートフォン」 の数量合計</t>
+    <rPh sb="0" eb="3">
+      <t>ショウヒンメイ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="17" eb="19">
+      <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>支払い方法が電子マネーの金額合計</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>日付が2025/11/03の金額合計</t>
+    <rPh sb="0" eb="2">
+      <t>ヒヅケ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="16" eb="18">
+      <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>条件</t>
+    <rPh sb="0" eb="2">
+      <t>ジョウケン</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>スマートフォン</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>2025/11/03</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>電子マネー</t>
+    <rPh sb="0" eb="2">
+      <t>デンシ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>※C5を参照するか，DATE関数を使う</t>
+    <rPh sb="4" eb="6">
+      <t>サンショウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>カンスウ</t>
+    </rPh>
+    <rPh sb="17" eb="18">
+      <t>ツカ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>&gt;=20000</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>金額が20,000以上の数量合計</t>
+    <rPh sb="0" eb="2">
+      <t>キンガク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>イジョウ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>スウリョウ</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ゴウケイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>値</t>
     <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>スマートフォン</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>例２</t>
+      <t>アタイ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>桁数</t>
     <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>例３</t>
-    <rPh sb="0" eb="1">
-      <t>レイ</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>社員ID</t>
-  </si>
-  <si>
-    <t>氏名</t>
-  </si>
-  <si>
-    <t>部署</t>
-  </si>
-  <si>
-    <t>勤務日数</t>
-  </si>
-  <si>
-    <t>残業時間</t>
-  </si>
-  <si>
-    <t>E001</t>
-  </si>
-  <si>
-    <t>営業</t>
-  </si>
-  <si>
-    <t>E002</t>
-  </si>
-  <si>
-    <t>経理</t>
-  </si>
-  <si>
-    <t>E003</t>
-  </si>
-  <si>
-    <t>開発</t>
-  </si>
-  <si>
-    <t>E004</t>
-  </si>
-  <si>
-    <t>E005</t>
-  </si>
-  <si>
-    <t>E006</t>
-  </si>
-  <si>
-    <t>中村健</t>
-  </si>
-  <si>
-    <t>E007</t>
-  </si>
-  <si>
-    <t>E008</t>
-  </si>
-  <si>
-    <t>総務</t>
-  </si>
-  <si>
-    <t>E009</t>
-  </si>
-  <si>
-    <t>E010</t>
-  </si>
-  <si>
-    <t>練習内容</t>
-  </si>
-  <si>
-    <t>条件</t>
-  </si>
-  <si>
-    <t>使用関数例</t>
-  </si>
-  <si>
-    <t>結果</t>
-  </si>
-  <si>
-    <t>開発部の残業時間合計</t>
-  </si>
-  <si>
-    <t>経理部の勤務日数合計</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> =SUMIF(D3:D12,"営業",E3:E12)</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>営業部の勤務日数合計</t>
+      <t>ケタ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>スウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ROUND関数</t>
+    <rPh sb="5" eb="7">
+      <t>カンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ROUNDDOWN関数</t>
+    <rPh sb="9" eb="11">
+      <t>カンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>ROUNDUP関数</t>
+    <rPh sb="7" eb="9">
+      <t>カンスウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>学籍番号</t>
+    <rPh sb="0" eb="2">
+      <t>ガクセキ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>入学年度</t>
+    <rPh sb="0" eb="2">
+      <t>ニュウガク</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>ネンド</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>学部</t>
+    <rPh sb="0" eb="2">
+      <t>ガクブ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>学科番号</t>
+    <rPh sb="0" eb="2">
+      <t>ガッカ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>個人番号</t>
+    <rPh sb="0" eb="2">
+      <t>コジン</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>バンゴウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>23B3456</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>↑自分の学籍番号を入力してください</t>
+    <rPh sb="1" eb="3">
+      <t>ジブン</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ガクセキ</t>
+    </rPh>
+    <rPh sb="6" eb="8">
+      <t>バンゴウ</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ニュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>25A7123</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -329,10 +609,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="179" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
-    <numFmt numFmtId="181" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
+    <numFmt numFmtId="176" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
+    <numFmt numFmtId="177" formatCode="&quot;¥&quot;#,##0.00_);[Red]\(&quot;¥&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -369,8 +649,16 @@
       <family val="1"/>
       <charset val="128"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="UD Digi Kyokasho NP-R"/>
+      <family val="1"/>
+      <charset val="128"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +674,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,7 +748,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -471,28 +765,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -519,7 +810,21 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="桁区切り" xfId="1" builtinId="6"/>
@@ -825,7 +1130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="C15" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -842,28 +1147,28 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:10" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1472,7 +1777,7 @@
         <v>13</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G26" s="7">
         <v>80000</v>
@@ -1688,7 +1993,7 @@
   <dimension ref="B3:C9"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1698,10 +2003,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="13"/>
+      <c r="C3" s="21"/>
     </row>
     <row r="4" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
@@ -1769,55 +2074,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F9D3B08-C40F-4160-9DA9-F2F5816DEC96}">
   <dimension ref="B2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="8" max="8" width="21.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="4.25" customWidth="1"/>
+    <col min="8" max="8" width="29.5" customWidth="1"/>
+    <col min="9" max="9" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="F2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>72</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="3" spans="2:11" ht="21.95" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B3" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>58</v>
+      <c r="D3" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E3" s="4">
         <v>18</v>
@@ -1826,28 +2132,28 @@
         <v>11</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J3" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="1">
+        <v>55</v>
+      </c>
+      <c r="J3" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="11">
         <f>SUMIF(D3:D12,"営業",E3:E12)</f>
         <v>80</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>60</v>
+      <c r="D4" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="E4" s="4">
         <v>19</v>
@@ -1856,23 +2162,28 @@
         <v>3</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="J4" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="11">
+        <f>SUMIF(D3:D12,"開発",F3:F12)</f>
+        <v>15</v>
+      </c>
     </row>
     <row r="5" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>62</v>
+      <c r="D5" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="E5" s="4">
         <v>23</v>
@@ -1881,23 +2192,28 @@
         <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+        <v>76</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="K5" s="11">
+        <f>SUMIF(E3:E12,"&gt;=20",F3:F12)</f>
+        <v>16</v>
+      </c>
     </row>
     <row r="6" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="4" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>58</v>
+      <c r="D6" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E6" s="4">
         <v>22</v>
@@ -1905,20 +2221,16 @@
       <c r="F6" s="4">
         <v>6</v>
       </c>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
     </row>
     <row r="7" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>58</v>
+      <c r="D7" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E7" s="4">
         <v>18</v>
@@ -1929,13 +2241,13 @@
     </row>
     <row r="8" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="E8" s="4">
         <v>19</v>
@@ -1946,13 +2258,13 @@
     </row>
     <row r="9" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="20" t="s">
-        <v>58</v>
+      <c r="D9" s="19" t="s">
+        <v>55</v>
       </c>
       <c r="E9" s="4">
         <v>22</v>
@@ -1963,13 +2275,13 @@
     </row>
     <row r="10" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B10" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="20" t="s">
-        <v>69</v>
+      <c r="D10" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="E10" s="4">
         <v>19</v>
@@ -1980,13 +2292,13 @@
     </row>
     <row r="11" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B11" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="20" t="s">
-        <v>60</v>
+      <c r="D11" s="19" t="s">
+        <v>57</v>
       </c>
       <c r="E11" s="4">
         <v>18</v>
@@ -1997,13 +2309,13 @@
     </row>
     <row r="12" spans="2:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B12" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>62</v>
+      <c r="D12" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="E12" s="4">
         <v>23</v>
@@ -2020,46 +2332,306 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8D8DC-46F7-4026-B0E5-5D87A029801D}">
-  <dimension ref="B2:C5"/>
+  <dimension ref="B2:E7"/>
   <sheetViews>
     <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="12"/>
-    </row>
-    <row r="3" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="11"/>
-    </row>
-    <row r="4" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D3" s="12"/>
+    </row>
+    <row r="4" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="11"/>
-    </row>
-    <row r="5" spans="2:3" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+        <v>80</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="11">
+        <f>SUMIF(注文履歴!F4:F33,"スマートフォン",注文履歴!H4:H33)</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C5" s="11"/>
+        <v>82</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="11">
+        <f>SUMIF(注文履歴!D4:D33,C5,注文履歴!I4:I33)</f>
+        <v>1921000</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="11">
+        <f>SUMIF(注文履歴!I4:I33,"&gt;=20000",注文履歴!H4:H33)</f>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="11">
+        <f>SUMIF(注文履歴!J4:J33,"電子マネー",注文履歴!I4:I33)</f>
+        <v>1096000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8F108E-C207-46ED-932A-DAF1179ED7BA}">
+  <dimension ref="B2:F7"/>
+  <sheetViews>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="16.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="1">
+        <v>140.178</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <f>ROUND(B3,C3)</f>
+        <v>140</v>
+      </c>
+      <c r="E3" s="11">
+        <f>ROUNDDOWN(B3,C3)</f>
+        <v>140</v>
+      </c>
+      <c r="F3" s="11">
+        <f>ROUNDUP(B3,C3)</f>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="1">
+        <v>140.178</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11">
+        <f t="shared" ref="D4:D7" si="0">ROUND(B4,C4)</f>
+        <v>140.19999999999999</v>
+      </c>
+      <c r="E4" s="11">
+        <f t="shared" ref="E4:E7" si="1">ROUNDDOWN(B4,C4)</f>
+        <v>140.1</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F7" si="2">ROUNDUP(B4,C4)</f>
+        <v>140.19999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="1">
+        <v>140.178</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="11">
+        <f t="shared" si="0"/>
+        <v>140.18</v>
+      </c>
+      <c r="E5" s="11">
+        <f t="shared" si="1"/>
+        <v>140.16999999999999</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="2"/>
+        <v>140.17999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="1">
+        <v>140.178</v>
+      </c>
+      <c r="C6" s="4">
+        <v>-1</v>
+      </c>
+      <c r="D6" s="11">
+        <f t="shared" si="0"/>
+        <v>140</v>
+      </c>
+      <c r="E6" s="11">
+        <f t="shared" si="1"/>
+        <v>140</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B7" s="1">
+        <v>140.178</v>
+      </c>
+      <c r="C7" s="4">
+        <v>-2</v>
+      </c>
+      <c r="D7" s="11">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="E7" s="11">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54B8CC66-7399-475D-AB8B-0D575B68A4F6}">
+  <dimension ref="B2:F5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="2" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <f>LEFT(B3,2)</f>
+        <v>23</v>
+      </c>
+      <c r="D3" s="8" t="str">
+        <f>MID(B3,3,1)</f>
+        <v>B</v>
+      </c>
+      <c r="E3" s="8" t="str">
+        <f>MID(B3,4,1)</f>
+        <v>3</v>
+      </c>
+      <c r="F3" s="8" t="str">
+        <f>RIGHT(B3,3)</f>
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="8" t="str">
+        <f>LEFT(B4,2)</f>
+        <v>25</v>
+      </c>
+      <c r="D4" s="8" t="str">
+        <f>MID(B4,3,1)</f>
+        <v>A</v>
+      </c>
+      <c r="E4" s="8" t="str">
+        <f>MID(B4,4,1)</f>
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="str">
+        <f>RIGHT(B4,3)</f>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="25" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>